<commit_message>
Added Code to get the AverageNumberOfRidersForEachDayOfTheWeek to work
It Works! It Works! WOOOOOOOOOOOOOOOOT!
</commit_message>
<xml_diff>
--- a/Source/Data/processed/average_ridership_2023.xlsx
+++ b/Source/Data/processed/average_ridership_2023.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Average Ridership" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Day of the Week</t>
   </si>
@@ -47,16 +47,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,27 +67,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -101,16 +81,29 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Day of the Week"/>
+    <tableColumn id="2" name="Average Ridership" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,9 +396,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -416,59 +413,62 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>134782.7700320513</v>
+      <c r="B2" s="1">
+        <v>3234786.480769231</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>155967.8076923077</v>
+      <c r="B3" s="1">
+        <v>3743227.384615385</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>159834.2540064103</v>
+      <c r="B4" s="1">
+        <v>3836022.096153846</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>157507.1137820513</v>
+      <c r="B5" s="1">
+        <v>3780170.730769231</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>145210.0953525641</v>
+      <c r="B6" s="1">
+        <v>3485042.288461538</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>98843.95833333333</v>
+      <c r="B7" s="1">
+        <v>2372255</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>78887.65932336742</v>
+      <c r="B8" s="1">
+        <v>1891815.377358491</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>